<commit_message>
changed 'name' column to 'activity_name' column to stop clash with native attribute
</commit_message>
<xml_diff>
--- a/test/exampledata2.xlsx
+++ b/test/exampledata2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\local\python\giganttic\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C13C4CBA-2C73-49F9-854F-1199317119A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D793E83-366C-4078-9622-4D47833120CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31095" yWindow="2625" windowWidth="21600" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,9 +56,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
     <t>T0</t>
   </si>
   <si>
@@ -126,6 +123,9 @@
   </si>
   <si>
     <t>Deborah</t>
+  </si>
+  <si>
+    <t>activity_name</t>
   </si>
 </sst>
 </file>
@@ -453,7 +453,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,36 +467,36 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="H1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1">
         <v>45017</v>
@@ -517,15 +517,15 @@
         <v>10</v>
       </c>
       <c r="I2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1">
         <v>45017</v>
@@ -546,15 +546,15 @@
         <v>1.3</v>
       </c>
       <c r="I3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1">
         <v>45383</v>
@@ -575,15 +575,15 @@
         <v>100</v>
       </c>
       <c r="I4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1">
         <v>46113</v>
@@ -604,7 +604,7 @@
         <v>100</v>
       </c>
       <c r="I5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -612,7 +612,7 @@
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="1">
         <v>45017</v>
@@ -633,7 +633,7 @@
         <v>10</v>
       </c>
       <c r="I6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -641,7 +641,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7" s="1">
         <v>45748</v>
@@ -659,7 +659,7 @@
         <v>10</v>
       </c>
       <c r="I7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -667,7 +667,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8" s="1">
         <v>45748</v>
@@ -685,7 +685,7 @@
         <v>50</v>
       </c>
       <c r="I8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -693,7 +693,7 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="1">
         <v>45383</v>
@@ -714,7 +714,7 @@
         <v>55</v>
       </c>
       <c r="I9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>